<commit_message>
refactor(BCHEP-542): contractor import process
</commit_message>
<xml_diff>
--- a/scripts/contractor_import/esp_contractor_data.xlsx
+++ b/scripts/contractor_import/esp_contractor_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\siegleda\workspace\bc-emli-application-sys\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\siegleda\workspace\bc-emli-application-sys\scripts\contractor_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1795E-7694-41C7-A940-DDC7FB2A9D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71306643-8CED-4123-BF89-A317B650B96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="3405" windowWidth="29040" windowHeight="15720" xr2:uid="{F7AEAF2D-E846-44F6-B64F-8752269011DB}"/>
   </bookViews>
@@ -245,9 +245,6 @@
     <t>Asbestos/Vermiculite remediation, Mould remediation</t>
   </si>
   <si>
-    <t>marklandelectric@gmail.com</t>
-  </si>
-  <si>
     <t>Markland</t>
   </si>
   <si>
@@ -267,9 +264,6 @@
   </si>
   <si>
     <t>https://www.facebook.com/matrixindustriesinc/</t>
-  </si>
-  <si>
-    <t>Pridegasheating@yahoo.ca</t>
   </si>
   <si>
     <t>Jabarjang</t>
@@ -297,9 +291,6 @@
 2024-08-29: (NK) 1st review complete, webinar sent.</t>
   </si>
   <si>
-    <t>valleysidehvac@gmail.com</t>
-  </si>
-  <si>
     <t>Salekin</t>
   </si>
   <si>
@@ -320,9 +311,6 @@
   <si>
     <t>2025-09-22: (NK) Approved, contractor emailed webinar viewed._x000D_
 2025-09-15: (MS) 1st review complete, webinar sent.</t>
-  </si>
-  <si>
-    <t>dan@authenticinstallations.com</t>
   </si>
   <si>
     <t>Devries</t>
@@ -356,9 +344,6 @@
 2025-08-13: (MS) 1st review IP, IR sent for BL, GST, WorkSafeBC, COI, TSBC</t>
   </si>
   <si>
-    <t>Devon@harbourhazmat.ca</t>
-  </si>
-  <si>
     <t>Harbour Hazmat Inc</t>
   </si>
   <si>
@@ -399,13 +384,28 @@
   </si>
   <si>
     <t>Unique Code</t>
+  </si>
+  <si>
+    <t>test.example2@fakeemail.com</t>
+  </si>
+  <si>
+    <t>test.example3@fakeemail.com</t>
+  </si>
+  <si>
+    <t>test.example1@fakeemail.com</t>
+  </si>
+  <si>
+    <t>test.example4@fakeemail.com</t>
+  </si>
+  <si>
+    <t>test.example5@fakeemail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +418,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -437,14 +445,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
@@ -1294,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0562C1C5-C18A-4252-B69E-EE1F89A3B323}">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,18 +1464,18 @@
         <v>36</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>37</v>
@@ -1479,31 +1490,31 @@
         <v>161621</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>39</v>
@@ -1512,19 +1523,19 @@
         <v>4</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>40</v>
@@ -1542,7 +1553,7 @@
         <v>42</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>43</v>
@@ -1551,24 +1562,24 @@
         <v>44</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AK2" s="1">
         <v>2012</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>69</v>
+      <c r="A3" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>37</v>
@@ -1580,34 +1591,34 @@
         <v>727216418</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>39</v>
@@ -1616,10 +1627,10 @@
         <v>1</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>39</v>
@@ -1634,7 +1645,7 @@
         <v>56</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>43</v>
@@ -1643,24 +1654,24 @@
         <v>44</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AK3" s="1">
         <v>2023</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>94</v>
+      <c r="A4" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>37</v>
@@ -1675,10 +1686,10 @@
         <v>817480247</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>55</v>
@@ -1687,19 +1698,19 @@
         <v>5915816</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>38</v>
@@ -1711,10 +1722,10 @@
         <v>10</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>40</v>
@@ -1729,7 +1740,7 @@
         <v>38</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AH4" s="1" t="s">
         <v>43</v>
@@ -1738,24 +1749,24 @@
         <v>51</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="AK4" s="1">
         <v>2013</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>86</v>
+      <c r="A5" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>37</v>
@@ -1770,28 +1781,28 @@
         <v>2531</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>38</v>
@@ -1803,10 +1814,10 @@
         <v>2</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>40</v>
@@ -1824,7 +1835,7 @@
         <v>48</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AH5" s="1" t="s">
         <v>43</v>
@@ -1833,18 +1844,18 @@
         <v>44</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AK5" s="1">
         <v>2013</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>104</v>
+      <c r="A6" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -1865,19 +1876,19 @@
         <v>4842</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>68</v>
@@ -1886,19 +1897,19 @@
         <v>41</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>50</v>
@@ -1907,7 +1918,7 @@
         <v>7</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>61</v>
@@ -1916,10 +1927,10 @@
         <v>67</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>39</v>
@@ -1934,7 +1945,7 @@
         <v>52</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AH6" s="1" t="s">
         <v>43</v>
@@ -1943,20 +1954,27 @@
         <v>44</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AK6" s="1">
         <v>2022</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EC93A6BC-7775-41C1-8EBE-04CB0AAECF39}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{A8FCB8E1-F709-41BA-9E46-CF89928E7DCA}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{3ECF46B0-B5EF-4439-869B-316D91F475C8}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{53BF5B9D-C4BB-4638-B2D4-99D6292C60A2}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{C644B2E0-2D98-4ED4-99BC-0390F0FD35D0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>